<commit_message>
work with Excel data
1) ExcelDataTests - ome tests to work with Excel
2) ExcelDataProvider - class to work with excelFile
3) ExcelPageNumber - enum class with names of sheets
4) ExcelReader - class with configuration

+ some fixes
1. Change path to classes
2. Change annotation before and after for beforeMethod and afterMethod
3. Add setters in BooksData class
4.
</commit_message>
<xml_diff>
--- a/src/main/resources/names_data.xlsx
+++ b/src/main/resources/names_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/golikovyurijalexandrovich/IdeaProjects/ToolsQA/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5640553-A477-4948-8963-FCA838904CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE09B44-FAD5-D346-B63E-D64116AD398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{27E0C8DA-56E8-584E-AA53-F870DD78C654}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16500" xr2:uid="{27E0C8DA-56E8-584E-AA53-F870DD78C654}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E6BF0A-0B07-E546-AF09-645B5B5B7310}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -508,6 +508,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -515,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C1E202-8263-BA41-A48B-1BD8C5101F2B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>